<commit_message>
Half of Air Quality Scalation
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sdk/Desktop/UGA_proj/DS2_P1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tango\Desktop\Projects\Project1\DS2_P1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A6438F7-B4D6-EA43-BEB7-6AE2D8CCB13F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C007E7B-9EFE-4D70-A05F-9B7FBEA46A92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="3" xr2:uid="{148821D6-7D66-074A-A975-42F1D73B03D7}"/>
+    <workbookView xWindow="20610" yWindow="3045" windowWidth="17790" windowHeight="12555" activeTab="2" xr2:uid="{148821D6-7D66-074A-A975-42F1D73B03D7}"/>
   </bookViews>
   <sheets>
     <sheet name="AutoMPG" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="30">
   <si>
     <t>Linear Regression</t>
   </si>
@@ -127,6 +127,9 @@
   </si>
   <si>
     <t>Cylinders, ModelYear</t>
+  </si>
+  <si>
+    <t>Time, PT08.S1, PT08.S2, AH</t>
   </si>
 </sst>
 </file>
@@ -134,7 +137,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="174" formatCode="0.000000"/>
+    <numFmt numFmtId="164" formatCode="0.000000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -187,17 +190,17 @@
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="174" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -514,359 +517,359 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47F1CD96-39E2-A543-849F-085C8A38E72C}">
   <dimension ref="C4:P13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K8" sqref="K7:K8"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.1640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="23.1640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="24.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="24.875" bestFit="1" customWidth="1"/>
     <col min="13" max="16" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:16" ht="19" x14ac:dyDescent="0.25">
-      <c r="C4" s="2" t="s">
+    <row r="4" spans="3:16" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C4" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="2" t="s">
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-      <c r="O4" s="2"/>
-      <c r="P4" s="2"/>
-    </row>
-    <row r="5" spans="3:16" ht="19" x14ac:dyDescent="0.25">
-      <c r="C5" s="3" t="s">
+      <c r="L4" s="6"/>
+      <c r="M4" s="6"/>
+      <c r="N4" s="6"/>
+      <c r="O4" s="6"/>
+      <c r="P4" s="6"/>
+    </row>
+    <row r="5" spans="3:16" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="H5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3" t="s">
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="L5" s="3" t="s">
+      <c r="L5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="M5" s="3" t="s">
+      <c r="M5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="N5" s="3" t="s">
+      <c r="N5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="O5" s="3" t="s">
+      <c r="O5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="P5" s="3" t="s">
+      <c r="P5" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="3:16" ht="19" x14ac:dyDescent="0.25">
-      <c r="C6" s="3" t="s">
+    <row r="6" spans="3:16" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C6" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="3">
         <v>0.80766300000000002</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="3">
         <v>0.806674</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G6" s="2">
         <v>-198.43</v>
       </c>
-      <c r="H6" s="4">
+      <c r="H6" s="2">
         <v>-191.36</v>
       </c>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3" t="s">
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="L6" s="3" t="s">
+      <c r="L6" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="M6" s="5">
+      <c r="M6" s="3">
         <v>0.80362069999999997</v>
       </c>
-      <c r="N6" s="5">
+      <c r="N6" s="3">
         <v>0.80311710000000003</v>
       </c>
-      <c r="O6" s="4">
+      <c r="O6" s="2">
         <v>197.08059791597</v>
       </c>
-      <c r="P6" s="4">
+      <c r="P6" s="2">
         <v>201.804206789971</v>
       </c>
     </row>
-    <row r="7" spans="3:16" ht="19" x14ac:dyDescent="0.25">
-      <c r="C7" s="3" t="s">
+    <row r="7" spans="3:16" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C7" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="3">
         <v>0.82715499999999997</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="3">
         <v>0.82536900000000002</v>
       </c>
-      <c r="G7" s="4">
+      <c r="G7" s="2">
         <v>-195.69399999999999</v>
       </c>
-      <c r="H7" s="4">
+      <c r="H7" s="2">
         <v>-183.911</v>
       </c>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3" t="s">
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="L7" s="3" t="s">
+      <c r="L7" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="M7" s="5">
+      <c r="M7" s="3">
         <v>0.80362299999999998</v>
       </c>
-      <c r="N7" s="5">
+      <c r="N7" s="3">
         <v>0.80311949999999999</v>
       </c>
-      <c r="O7" s="4">
+      <c r="O7" s="2">
         <v>197.07922478145201</v>
       </c>
-      <c r="P7" s="4">
+      <c r="P7" s="2">
         <v>201.80283365545301</v>
       </c>
     </row>
-    <row r="8" spans="3:16" ht="19" x14ac:dyDescent="0.25">
-      <c r="C8" s="3" t="s">
+    <row r="8" spans="3:16" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C8" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="3">
         <v>0.82715499999999997</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="3">
         <v>0.82581899999999997</v>
       </c>
-      <c r="G8" s="4">
+      <c r="G8" s="2">
         <v>-195.84</v>
       </c>
-      <c r="H8" s="4">
+      <c r="H8" s="2">
         <v>-194.15600000000001</v>
       </c>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3" t="s">
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="L8" s="3" t="s">
+      <c r="L8" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="M8" s="5">
+      <c r="M8" s="3">
         <v>0.80273649999999996</v>
       </c>
-      <c r="N8" s="5">
+      <c r="N8" s="3">
         <v>0.80223069999999996</v>
       </c>
-      <c r="O8" s="4">
+      <c r="O8" s="2">
         <v>197.18740126518401</v>
       </c>
-      <c r="P8" s="4">
+      <c r="P8" s="2">
         <v>201.91101013918501</v>
       </c>
     </row>
-    <row r="9" spans="3:16" ht="19" x14ac:dyDescent="0.25">
-      <c r="C9" s="3" t="s">
+    <row r="9" spans="3:16" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C9" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9" s="3">
         <v>0.855402</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="3">
         <v>0.853908</v>
       </c>
-      <c r="G9" s="4">
+      <c r="G9" s="2">
         <v>-186.21199999999999</v>
       </c>
-      <c r="H9" s="4">
+      <c r="H9" s="2">
         <v>-174.428</v>
       </c>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3" t="s">
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="L9" s="3" t="s">
+      <c r="L9" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="M9" s="5">
+      <c r="M9" s="3">
         <v>0.84790180000000004</v>
       </c>
-      <c r="N9" s="5">
+      <c r="N9" s="3">
         <v>0.84751180000000004</v>
       </c>
-      <c r="O9" s="4">
+      <c r="O9" s="2">
         <v>173.732546811715</v>
       </c>
-      <c r="P9" s="4">
+      <c r="P9" s="2">
         <v>178.456155685716</v>
       </c>
     </row>
-    <row r="10" spans="3:16" ht="19" x14ac:dyDescent="0.25">
-      <c r="C10" s="3" t="s">
+    <row r="10" spans="3:16" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="3">
         <v>0.85837600000000003</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F10" s="3">
         <v>0.85691200000000001</v>
       </c>
-      <c r="G10" s="4">
+      <c r="G10" s="2">
         <v>-182.40600000000001</v>
       </c>
-      <c r="H10" s="4">
+      <c r="H10" s="2">
         <v>-170.62200000000001</v>
       </c>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3" t="s">
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="L10" s="3"/>
-      <c r="M10" s="3"/>
-      <c r="N10" s="3"/>
-      <c r="O10" s="3"/>
-      <c r="P10" s="3"/>
-    </row>
-    <row r="11" spans="3:16" ht="19" x14ac:dyDescent="0.25">
-      <c r="C11" s="3" t="s">
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+    </row>
+    <row r="11" spans="3:16" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E11" s="5">
+      <c r="E11" s="3">
         <v>0.85812100000000002</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F11" s="3">
         <v>0.85665500000000006</v>
       </c>
-      <c r="G11" s="4">
+      <c r="G11" s="2">
         <v>-182.47499999999999</v>
       </c>
-      <c r="H11" s="4">
+      <c r="H11" s="2">
         <v>-170.69200000000001</v>
       </c>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3" t="s">
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="L11" s="3"/>
-      <c r="M11" s="3"/>
-      <c r="N11" s="3"/>
-      <c r="O11" s="3"/>
-      <c r="P11" s="3"/>
-    </row>
-    <row r="12" spans="3:16" ht="19" x14ac:dyDescent="0.25">
-      <c r="C12" s="3" t="s">
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+    </row>
+    <row r="12" spans="3:16" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C12" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E12" s="5">
+      <c r="E12" s="3">
         <v>0.86060700000000001</v>
       </c>
-      <c r="F12" s="5">
+      <c r="F12" s="3">
         <v>0.85843499999999995</v>
       </c>
-      <c r="G12" s="4">
+      <c r="G12" s="2">
         <v>-179.691</v>
       </c>
-      <c r="H12" s="4">
+      <c r="H12" s="2">
         <v>-163.19399999999999</v>
       </c>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3" t="s">
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="L12" s="3"/>
-      <c r="M12" s="3"/>
-      <c r="N12" s="3"/>
-      <c r="O12" s="3"/>
-      <c r="P12" s="3"/>
-    </row>
-    <row r="13" spans="3:16" ht="19" x14ac:dyDescent="0.25">
-      <c r="C13" s="3" t="s">
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+    </row>
+    <row r="13" spans="3:16" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C13" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E13" s="5">
+      <c r="E13" s="3">
         <v>0.85847399999999996</v>
       </c>
-      <c r="F13" s="5">
+      <c r="F13" s="3">
         <v>0.85664099999999999</v>
       </c>
-      <c r="G13" s="4">
+      <c r="G13" s="2">
         <v>-185.19300000000001</v>
       </c>
-      <c r="H13" s="4">
+      <c r="H13" s="2">
         <v>-174.56399999999999</v>
       </c>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
-      <c r="K13" s="3" t="s">
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="L13" s="3"/>
-      <c r="M13" s="3"/>
-      <c r="N13" s="3"/>
-      <c r="O13" s="3"/>
-      <c r="P13" s="3"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -885,275 +888,275 @@
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="27" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="27" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="28.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:18" ht="19" x14ac:dyDescent="0.25">
-      <c r="C4" s="2" t="s">
+    <row r="4" spans="3:18" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C4" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="2" t="s">
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-      <c r="O4" s="2"/>
-      <c r="P4" s="2"/>
-      <c r="Q4" s="2"/>
-      <c r="R4" s="2"/>
-    </row>
-    <row r="5" spans="3:18" ht="19" x14ac:dyDescent="0.25">
-      <c r="C5" s="3" t="s">
+      <c r="M4" s="6"/>
+      <c r="N4" s="6"/>
+      <c r="O4" s="6"/>
+      <c r="P4" s="6"/>
+      <c r="Q4" s="6"/>
+      <c r="R4" s="6"/>
+    </row>
+    <row r="5" spans="3:18" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="H5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I5" s="3" t="s">
+      <c r="I5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3" t="s">
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="M5" s="3" t="s">
+      <c r="M5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="N5" s="3" t="s">
+      <c r="N5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="O5" s="3" t="s">
+      <c r="O5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="P5" s="3" t="s">
+      <c r="P5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="Q5" s="3" t="s">
+      <c r="Q5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="R5" s="3" t="s">
+      <c r="R5" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="3:18" ht="19" x14ac:dyDescent="0.25">
-      <c r="C6" s="3" t="s">
+    <row r="6" spans="3:18" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C6" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3" t="s">
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="M6" s="3"/>
-      <c r="N6" s="3"/>
-      <c r="O6" s="3"/>
-      <c r="P6" s="3"/>
-      <c r="Q6" s="3"/>
-      <c r="R6" s="3"/>
-    </row>
-    <row r="7" spans="3:18" ht="19" x14ac:dyDescent="0.25">
-      <c r="C7" s="3" t="s">
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="1"/>
+    </row>
+    <row r="7" spans="3:18" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C7" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3" t="s">
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="M7" s="3"/>
-      <c r="N7" s="3"/>
-      <c r="O7" s="3"/>
-      <c r="P7" s="3"/>
-      <c r="Q7" s="3"/>
-      <c r="R7" s="3"/>
-    </row>
-    <row r="8" spans="3:18" ht="19" x14ac:dyDescent="0.25">
-      <c r="C8" s="3" t="s">
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1"/>
+    </row>
+    <row r="8" spans="3:18" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C8" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3" t="s">
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="M8" s="3"/>
-      <c r="N8" s="3"/>
-      <c r="O8" s="3"/>
-      <c r="P8" s="3"/>
-      <c r="Q8" s="3"/>
-      <c r="R8" s="3"/>
-    </row>
-    <row r="9" spans="3:18" ht="19" x14ac:dyDescent="0.25">
-      <c r="C9" s="3" t="s">
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1"/>
+    </row>
+    <row r="9" spans="3:18" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C9" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
-      <c r="L9" s="3" t="s">
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="M9" s="3"/>
-      <c r="N9" s="3"/>
-      <c r="O9" s="3"/>
-      <c r="P9" s="3"/>
-      <c r="Q9" s="3"/>
-      <c r="R9" s="3"/>
-    </row>
-    <row r="10" spans="3:18" ht="19" x14ac:dyDescent="0.25">
-      <c r="C10" s="3" t="s">
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="1"/>
+    </row>
+    <row r="10" spans="3:18" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="3" t="s">
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="M10" s="3"/>
-      <c r="N10" s="3"/>
-      <c r="O10" s="3"/>
-      <c r="P10" s="3"/>
-      <c r="Q10" s="3"/>
-      <c r="R10" s="3"/>
-    </row>
-    <row r="11" spans="3:18" ht="19" x14ac:dyDescent="0.25">
-      <c r="C11" s="3" t="s">
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
+      <c r="R10" s="1"/>
+    </row>
+    <row r="11" spans="3:18" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
-      <c r="L11" s="3" t="s">
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="M11" s="3"/>
-      <c r="N11" s="3"/>
-      <c r="O11" s="3"/>
-      <c r="P11" s="3"/>
-      <c r="Q11" s="3"/>
-      <c r="R11" s="3"/>
-    </row>
-    <row r="12" spans="3:18" ht="19" x14ac:dyDescent="0.25">
-      <c r="C12" s="3" t="s">
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
+      <c r="R11" s="1"/>
+    </row>
+    <row r="12" spans="3:18" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C12" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
-      <c r="L12" s="3" t="s">
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="M12" s="3"/>
-      <c r="N12" s="3"/>
-      <c r="O12" s="3"/>
-      <c r="P12" s="3"/>
-      <c r="Q12" s="3"/>
-      <c r="R12" s="3"/>
-    </row>
-    <row r="13" spans="3:18" ht="19" x14ac:dyDescent="0.25">
-      <c r="C13" s="3" t="s">
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1"/>
+      <c r="R12" s="1"/>
+    </row>
+    <row r="13" spans="3:18" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C13" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
-      <c r="K13" s="3"/>
-      <c r="L13" s="3" t="s">
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="M13" s="3"/>
-      <c r="N13" s="3"/>
-      <c r="O13" s="3"/>
-      <c r="P13" s="3"/>
-      <c r="Q13" s="3"/>
-      <c r="R13" s="3"/>
-    </row>
-    <row r="14" spans="3:18" ht="21" x14ac:dyDescent="0.25">
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="6"/>
-      <c r="K14" s="6"/>
-      <c r="L14" s="6"/>
-      <c r="M14" s="6"/>
-      <c r="N14" s="6"/>
-      <c r="O14" s="6"/>
-      <c r="P14" s="6"/>
-      <c r="Q14" s="6"/>
-      <c r="R14" s="6"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+      <c r="Q13" s="1"/>
+      <c r="R13" s="1"/>
+    </row>
+    <row r="14" spans="3:18" ht="21" x14ac:dyDescent="0.35">
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
+      <c r="L14" s="4"/>
+      <c r="M14" s="4"/>
+      <c r="N14" s="4"/>
+      <c r="O14" s="4"/>
+      <c r="P14" s="4"/>
+      <c r="Q14" s="4"/>
+      <c r="R14" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1168,279 +1171,309 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61589931-3425-604A-8C2E-7C1B3F69C4DF}">
   <dimension ref="C4:P13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="21" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="27" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="10" width="10.83203125" style="6"/>
-    <col min="11" max="11" width="27" style="6" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="53.5" style="6" bestFit="1" customWidth="1"/>
-    <col min="13" max="16" width="13.1640625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="27" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.625" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="10" width="10.875" style="4"/>
+    <col min="11" max="11" width="27" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="53.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="16" width="13.125" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:16" ht="19" x14ac:dyDescent="0.25">
-      <c r="C4" s="2" t="s">
+    <row r="4" spans="3:16" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C4" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="2" t="s">
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-      <c r="O4" s="2"/>
-      <c r="P4" s="2"/>
-    </row>
-    <row r="5" spans="3:16" ht="19" x14ac:dyDescent="0.25">
-      <c r="C5" s="3" t="s">
+      <c r="L4" s="6"/>
+      <c r="M4" s="6"/>
+      <c r="N4" s="6"/>
+      <c r="O4" s="6"/>
+      <c r="P4" s="6"/>
+    </row>
+    <row r="5" spans="3:16" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="H5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3" t="s">
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="L5" s="3" t="s">
+      <c r="L5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="M5" s="3" t="s">
+      <c r="M5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="N5" s="3" t="s">
+      <c r="N5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="O5" s="3" t="s">
+      <c r="O5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="P5" s="3" t="s">
+      <c r="P5" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="3:16" ht="19" x14ac:dyDescent="0.25">
-      <c r="C6" s="3" t="s">
+    <row r="6" spans="3:16" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C6" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3" t="s">
+      <c r="D6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0.954399</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0.95437899999999998</v>
+      </c>
+      <c r="G6" s="1">
+        <v>-10270.700000000001</v>
+      </c>
+      <c r="H6" s="1">
+        <v>-10243.200000000001</v>
+      </c>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="L6" s="3" t="s">
+      <c r="L6" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="M6" s="5">
+      <c r="M6" s="3">
         <v>0.95823199999999997</v>
       </c>
-      <c r="N6" s="5">
+      <c r="N6" s="3">
         <v>0.95822200000000002</v>
       </c>
-      <c r="O6" s="4">
+      <c r="O6" s="2">
         <v>15312.96</v>
       </c>
-      <c r="P6" s="4">
+      <c r="P6" s="2">
         <v>15329.45</v>
       </c>
     </row>
-    <row r="7" spans="3:16" ht="19" x14ac:dyDescent="0.25">
-      <c r="C7" s="3" t="s">
+    <row r="7" spans="3:16" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C7" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3" t="s">
+      <c r="D7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0.94883899999999999</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0.95437300000000003</v>
+      </c>
+      <c r="G7" s="1">
+        <v>-10268.700000000001</v>
+      </c>
+      <c r="H7" s="1">
+        <v>-10235.700000000001</v>
+      </c>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="L7" s="3" t="s">
+      <c r="L7" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="M7" s="5">
+      <c r="M7" s="3">
         <v>0.95823199999999997</v>
       </c>
-      <c r="N7" s="5">
+      <c r="N7" s="3">
         <v>0.95822200000000002</v>
       </c>
-      <c r="O7" s="4">
+      <c r="O7" s="2">
         <v>15312.96</v>
       </c>
-      <c r="P7" s="4">
+      <c r="P7" s="2">
         <v>15329.45</v>
       </c>
     </row>
-    <row r="8" spans="3:16" ht="19" x14ac:dyDescent="0.25">
-      <c r="C8" s="3" t="s">
+    <row r="8" spans="3:16" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C8" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3" t="s">
+      <c r="D8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0.954399</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0.95437899999999998</v>
+      </c>
+      <c r="G8" s="1">
+        <v>-10270.700000000001</v>
+      </c>
+      <c r="H8" s="1">
+        <v>-10243.200000000001</v>
+      </c>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="L8" s="3" t="s">
+      <c r="L8" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="M8" s="5">
+      <c r="M8" s="3">
         <v>0.958175</v>
       </c>
-      <c r="N8" s="5">
+      <c r="N8" s="3">
         <v>0.95816500000000004</v>
       </c>
-      <c r="O8" s="4">
+      <c r="O8" s="2">
         <v>15315.36</v>
       </c>
-      <c r="P8" s="4">
+      <c r="P8" s="2">
         <v>15331.84</v>
       </c>
     </row>
-    <row r="9" spans="3:16" ht="19" x14ac:dyDescent="0.25">
-      <c r="C9" s="3" t="s">
+    <row r="9" spans="3:16" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C9" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3" t="s">
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="L9" s="3" t="s">
+      <c r="L9" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="M9" s="5">
+      <c r="M9" s="3">
         <v>0.78669</v>
       </c>
-      <c r="N9" s="5">
+      <c r="N9" s="3">
         <v>0.78659500000000004</v>
       </c>
-      <c r="O9" s="4">
+      <c r="O9" s="2">
         <v>18251.89</v>
       </c>
-      <c r="P9" s="4">
+      <c r="P9" s="2">
         <v>18279.37</v>
       </c>
     </row>
-    <row r="10" spans="3:16" ht="19" x14ac:dyDescent="0.25">
-      <c r="C10" s="3" t="s">
+    <row r="10" spans="3:16" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3" t="s">
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="L10" s="3"/>
-      <c r="M10" s="3"/>
-      <c r="N10" s="3"/>
-      <c r="O10" s="3"/>
-      <c r="P10" s="3"/>
-    </row>
-    <row r="11" spans="3:16" ht="19" x14ac:dyDescent="0.25">
-      <c r="C11" s="3" t="s">
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+    </row>
+    <row r="11" spans="3:16" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3" t="s">
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="L11" s="3"/>
-      <c r="M11" s="3"/>
-      <c r="N11" s="3"/>
-      <c r="O11" s="3"/>
-      <c r="P11" s="3"/>
-    </row>
-    <row r="12" spans="3:16" ht="19" x14ac:dyDescent="0.25">
-      <c r="C12" s="3" t="s">
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+    </row>
+    <row r="12" spans="3:16" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C12" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3" t="s">
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="L12" s="3"/>
-      <c r="M12" s="3"/>
-      <c r="N12" s="3"/>
-      <c r="O12" s="3"/>
-      <c r="P12" s="3"/>
-    </row>
-    <row r="13" spans="3:16" ht="19" x14ac:dyDescent="0.25">
-      <c r="C13" s="3" t="s">
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+    </row>
+    <row r="13" spans="3:16" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C13" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
-      <c r="K13" s="3" t="s">
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="L13" s="3"/>
-      <c r="M13" s="3"/>
-      <c r="N13" s="3"/>
-      <c r="O13" s="3"/>
-      <c r="P13" s="3"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1455,317 +1488,317 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8437764-9FAD-294F-8661-784D2EAF8AB2}">
   <dimension ref="C4:P13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="37" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="37" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:16" ht="19" x14ac:dyDescent="0.25">
-      <c r="C4" s="2" t="s">
+    <row r="4" spans="3:16" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C4" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="2" t="s">
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-      <c r="O4" s="2"/>
-      <c r="P4" s="2"/>
-    </row>
-    <row r="5" spans="3:16" ht="19" x14ac:dyDescent="0.25">
-      <c r="C5" s="3" t="s">
+      <c r="L4" s="6"/>
+      <c r="M4" s="6"/>
+      <c r="N4" s="6"/>
+      <c r="O4" s="6"/>
+      <c r="P4" s="6"/>
+    </row>
+    <row r="5" spans="3:16" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="H5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3" t="s">
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="L5" s="3" t="s">
+      <c r="L5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="M5" s="3" t="s">
+      <c r="M5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="N5" s="3" t="s">
+      <c r="N5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="O5" s="3" t="s">
+      <c r="O5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="P5" s="3" t="s">
+      <c r="P5" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="3:16" ht="19" x14ac:dyDescent="0.25">
-      <c r="C6" s="3" t="s">
+    <row r="6" spans="3:16" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C6" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="1">
         <v>0.91245399999999999</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="1">
         <v>0.91170399999999996</v>
       </c>
-      <c r="G6" s="3">
+      <c r="G6" s="1">
         <v>-5794.62</v>
       </c>
-      <c r="H6" s="3">
+      <c r="H6" s="1">
         <v>-5772.39</v>
       </c>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3" t="s">
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="L6" s="3"/>
-      <c r="M6" s="3"/>
-      <c r="N6" s="3"/>
-      <c r="O6" s="3"/>
-      <c r="P6" s="3"/>
-    </row>
-    <row r="7" spans="3:16" ht="19" x14ac:dyDescent="0.25">
-      <c r="C7" s="3" t="s">
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+    </row>
+    <row r="7" spans="3:16" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C7" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="1">
         <v>0.91245399999999999</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="1">
         <v>0.91120199999999996</v>
       </c>
-      <c r="G7" s="3">
+      <c r="G7" s="1">
         <v>-5824.74</v>
       </c>
-      <c r="H7" s="3">
+      <c r="H7" s="1">
         <v>-5796.96</v>
       </c>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3" t="s">
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="L7" s="3"/>
-      <c r="M7" s="3"/>
-      <c r="N7" s="3"/>
-      <c r="O7" s="3"/>
-      <c r="P7" s="3"/>
-    </row>
-    <row r="8" spans="3:16" ht="19" x14ac:dyDescent="0.25">
-      <c r="C8" s="3" t="s">
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+    </row>
+    <row r="8" spans="3:16" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C8" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="1">
         <v>0.91245399999999999</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="1">
         <v>0.912354</v>
       </c>
-      <c r="G8" s="3">
+      <c r="G8" s="1">
         <v>-5794.62</v>
       </c>
-      <c r="H8" s="3">
+      <c r="H8" s="1">
         <v>-5772.39</v>
       </c>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3" t="s">
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="L8" s="3"/>
-      <c r="M8" s="3"/>
-      <c r="N8" s="3"/>
-      <c r="O8" s="3"/>
-      <c r="P8" s="3"/>
-    </row>
-    <row r="9" spans="3:16" ht="19" x14ac:dyDescent="0.25">
-      <c r="C9" s="7" t="s">
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+    </row>
+    <row r="9" spans="3:16" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C9" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E9" s="7">
+      <c r="E9" s="5">
         <v>0.93970399999999998</v>
       </c>
-      <c r="F9" s="7">
+      <c r="F9" s="5">
         <v>0.93957100000000005</v>
       </c>
-      <c r="G9" s="7">
+      <c r="G9" s="5">
         <v>-5399.97</v>
       </c>
-      <c r="H9" s="7">
+      <c r="H9" s="5">
         <v>-5277.73</v>
       </c>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3" t="s">
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="L9" s="3"/>
-      <c r="M9" s="3"/>
-      <c r="N9" s="3"/>
-      <c r="O9" s="3"/>
-      <c r="P9" s="3"/>
-    </row>
-    <row r="10" spans="3:16" ht="19" x14ac:dyDescent="0.25">
-      <c r="C10" s="3" t="s">
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+    </row>
+    <row r="10" spans="3:16" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="1">
         <v>0.93676899999999996</v>
       </c>
-      <c r="F10" s="3">
+      <c r="F10" s="1">
         <v>0.93672299999999997</v>
       </c>
-      <c r="G10" s="3">
+      <c r="G10" s="1">
         <v>-5489.73</v>
       </c>
-      <c r="H10" s="3">
+      <c r="H10" s="1">
         <v>-5445.28</v>
       </c>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3" t="s">
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="L10" s="3"/>
-      <c r="M10" s="3"/>
-      <c r="N10" s="3"/>
-      <c r="O10" s="3"/>
-      <c r="P10" s="3"/>
-    </row>
-    <row r="11" spans="3:16" ht="19" x14ac:dyDescent="0.25">
-      <c r="C11" s="3" t="s">
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+    </row>
+    <row r="11" spans="3:16" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11" s="1">
         <v>0.93785499999999999</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F11" s="3">
         <v>0.93779000000000001</v>
       </c>
-      <c r="G11" s="3">
+      <c r="G11" s="1">
         <v>-5465.23</v>
       </c>
-      <c r="H11" s="3">
+      <c r="H11" s="1">
         <v>-5404.11</v>
       </c>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3" t="s">
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="L11" s="3"/>
-      <c r="M11" s="3"/>
-      <c r="N11" s="3"/>
-      <c r="O11" s="3"/>
-      <c r="P11" s="3"/>
-    </row>
-    <row r="12" spans="3:16" ht="19" x14ac:dyDescent="0.25">
-      <c r="C12" s="3" t="s">
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+    </row>
+    <row r="12" spans="3:16" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C12" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E12" s="1">
         <v>0.93898800000000004</v>
       </c>
-      <c r="F12" s="3">
+      <c r="F12" s="1">
         <v>0.93887900000000002</v>
       </c>
-      <c r="G12" s="3">
+      <c r="G12" s="1">
         <v>-5435.66</v>
       </c>
-      <c r="H12" s="3">
+      <c r="H12" s="1">
         <v>-5335.65</v>
       </c>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3" t="s">
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="L12" s="3"/>
-      <c r="M12" s="3"/>
-      <c r="N12" s="3"/>
-      <c r="O12" s="3"/>
-      <c r="P12" s="3"/>
-    </row>
-    <row r="13" spans="3:16" ht="19" x14ac:dyDescent="0.25">
-      <c r="C13" s="3" t="s">
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+    </row>
+    <row r="13" spans="3:16" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C13" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E13" s="3">
+      <c r="E13" s="1">
         <v>0.93922600000000001</v>
       </c>
-      <c r="F13" s="3">
+      <c r="F13" s="1">
         <v>0.93910499999999997</v>
       </c>
-      <c r="G13" s="3">
+      <c r="G13" s="1">
         <v>-5456.74</v>
       </c>
-      <c r="H13" s="3">
+      <c r="H13" s="1">
         <v>-5428.06</v>
       </c>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
-      <c r="K13" s="3" t="s">
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="L13" s="3"/>
-      <c r="M13" s="3"/>
-      <c r="N13" s="3"/>
-      <c r="O13" s="3"/>
-      <c r="P13" s="3"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1784,29 +1817,29 @@
       <selection activeCell="A4" sqref="A4:XFD13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="4" spans="3:18" x14ac:dyDescent="0.2">
-      <c r="C4" s="1" t="s">
+    <row r="4" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C4" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="L4" s="1" t="s">
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="L4" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="M4" s="1"/>
-      <c r="N4" s="1"/>
-      <c r="O4" s="1"/>
-      <c r="P4" s="1"/>
-      <c r="Q4" s="1"/>
-      <c r="R4" s="1"/>
-    </row>
-    <row r="5" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="M4" s="7"/>
+      <c r="N4" s="7"/>
+      <c r="O4" s="7"/>
+      <c r="P4" s="7"/>
+      <c r="Q4" s="7"/>
+      <c r="R4" s="7"/>
+    </row>
+    <row r="5" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>8</v>
       </c>
@@ -1850,7 +1883,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="3:18" x14ac:dyDescent="0.2">
+    <row r="6" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>0</v>
       </c>
@@ -1858,7 +1891,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="3:18" x14ac:dyDescent="0.2">
+    <row r="7" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>1</v>
       </c>
@@ -1866,7 +1899,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="3:18" x14ac:dyDescent="0.2">
+    <row r="8" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>2</v>
       </c>
@@ -1874,7 +1907,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="3:18" x14ac:dyDescent="0.2">
+    <row r="9" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>3</v>
       </c>
@@ -1882,7 +1915,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="3:18" x14ac:dyDescent="0.2">
+    <row r="10" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
         <v>6</v>
       </c>
@@ -1890,7 +1923,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="3:18" x14ac:dyDescent="0.2">
+    <row r="11" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
         <v>7</v>
       </c>
@@ -1898,7 +1931,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="3:18" x14ac:dyDescent="0.2">
+    <row r="12" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
         <v>4</v>
       </c>
@@ -1906,7 +1939,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="3:18" x14ac:dyDescent="0.2">
+    <row r="13" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
         <v>5</v>
       </c>
@@ -1931,29 +1964,29 @@
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="4" spans="3:18" x14ac:dyDescent="0.2">
-      <c r="C4" s="1" t="s">
+    <row r="4" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C4" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="L4" s="1" t="s">
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="L4" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="M4" s="1"/>
-      <c r="N4" s="1"/>
-      <c r="O4" s="1"/>
-      <c r="P4" s="1"/>
-      <c r="Q4" s="1"/>
-      <c r="R4" s="1"/>
-    </row>
-    <row r="5" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="M4" s="7"/>
+      <c r="N4" s="7"/>
+      <c r="O4" s="7"/>
+      <c r="P4" s="7"/>
+      <c r="Q4" s="7"/>
+      <c r="R4" s="7"/>
+    </row>
+    <row r="5" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>8</v>
       </c>
@@ -1997,7 +2030,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="3:18" x14ac:dyDescent="0.2">
+    <row r="6" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>0</v>
       </c>
@@ -2005,7 +2038,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="3:18" x14ac:dyDescent="0.2">
+    <row r="7" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>1</v>
       </c>
@@ -2013,7 +2046,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="3:18" x14ac:dyDescent="0.2">
+    <row r="8" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>2</v>
       </c>
@@ -2021,7 +2054,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="3:18" x14ac:dyDescent="0.2">
+    <row r="9" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>3</v>
       </c>
@@ -2029,7 +2062,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="3:18" x14ac:dyDescent="0.2">
+    <row r="10" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
         <v>6</v>
       </c>
@@ -2037,7 +2070,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="3:18" x14ac:dyDescent="0.2">
+    <row r="11" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
         <v>7</v>
       </c>
@@ -2045,7 +2078,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="3:18" x14ac:dyDescent="0.2">
+    <row r="12" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
         <v>4</v>
       </c>
@@ -2053,7 +2086,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="3:18" x14ac:dyDescent="0.2">
+    <row r="13" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
         <v>5</v>
       </c>

</xml_diff>